<commit_message>
Strt note for 5rules.
</commit_message>
<xml_diff>
--- a/finance/聚宽/学习笔记/2008/roe.xlsx
+++ b/finance/聚宽/学习笔记/2008/roe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lianbche\Git\knowledge-map\finance\聚宽\学习笔记\2008\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCBCCF4-516F-45F6-8B92-EC40A2807390}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7073C9EE-2E80-44A8-9FAB-7B7D2F6AE359}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,7 +1017,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1197,6 +1197,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1358,9 +1370,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1716,14 +1730,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I182" sqref="I182"/>
+      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1764,7 +1777,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1799,7 +1812,7 @@
         <v>0.92941176470588205</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1869,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1904,7 +1917,7 @@
         <v>0.668627450980392</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1939,7 +1952,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1974,7 +1987,7 @@
         <v>0.90392156862745099</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2009,8 +2022,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -2044,7 +2057,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2079,8 +2092,8 @@
         <v>0.96862745098039205</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1">
-      <c r="A11" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -2114,7 +2127,7 @@
         <v>0.95686274509803904</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2149,7 +2162,7 @@
         <v>0.95098039215686203</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2184,7 +2197,7 @@
         <v>0.94313725490195999</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2219,7 +2232,7 @@
         <v>0.96274509803921504</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2254,8 +2267,8 @@
         <v>0.97254901960784301</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -2289,8 +2302,8 @@
         <v>0.96666666666666601</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -2324,7 +2337,7 @@
         <v>0.96078431372549</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2359,7 +2372,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2394,7 +2407,7 @@
         <v>0.98431372549019602</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2429,7 +2442,7 @@
         <v>0.97647058823529398</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2464,7 +2477,7 @@
         <v>0.77254901960784295</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2499,8 +2512,8 @@
         <v>0.623529411764705</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1">
-      <c r="A23" t="s">
+    <row r="23" spans="1:11">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -2604,7 +2617,7 @@
         <v>0.474509803921568</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2639,7 +2652,7 @@
         <v>0.831372549019607</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2674,7 +2687,7 @@
         <v>0.86470588235294099</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2709,7 +2722,7 @@
         <v>0.53725490196078396</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2744,7 +2757,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2779,7 +2792,7 @@
         <v>0.97058823529411697</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2849,7 +2862,7 @@
         <v>0.39803921568627398</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2884,8 +2897,8 @@
         <v>0.915686274509803</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1">
-      <c r="A34" t="s">
+    <row r="34" spans="1:11">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34">
@@ -2919,7 +2932,7 @@
         <v>0.97450980392156805</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2954,7 +2967,7 @@
         <v>0.96274509803921504</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2989,8 +3002,8 @@
         <v>0.74901960784313704</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1">
-      <c r="A37" t="s">
+    <row r="37" spans="1:11">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37">
@@ -3024,8 +3037,8 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1">
-      <c r="A38" t="s">
+    <row r="38" spans="1:11">
+      <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B38">
@@ -3059,7 +3072,7 @@
         <v>0.63529411764705801</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3094,8 +3107,8 @@
         <v>0.94313725490195999</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1">
-      <c r="A40" t="s">
+    <row r="40" spans="1:11">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40">
@@ -3129,7 +3142,7 @@
         <v>0.95686274509803904</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -3199,7 +3212,7 @@
         <v>0.29411764705882298</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3234,7 +3247,7 @@
         <v>0.67647058823529405</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3269,7 +3282,7 @@
         <v>0.53333333333333299</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3304,8 +3317,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1">
-      <c r="A46" t="s">
+    <row r="46" spans="1:11">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46">
@@ -3339,7 +3352,7 @@
         <v>0.96862745098039205</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -3374,7 +3387,7 @@
         <v>0.98823529411764699</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3409,7 +3422,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -3444,7 +3457,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3479,7 +3492,7 @@
         <v>0.98823529411764699</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3514,7 +3527,7 @@
         <v>0.97843137254901902</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3549,7 +3562,7 @@
         <v>0.87254901960784303</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -3584,7 +3597,7 @@
         <v>0.98823529411764699</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3619,8 +3632,8 @@
         <v>0.96470588235294097</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1">
-      <c r="A55" t="s">
+    <row r="55" spans="1:11">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B55">
@@ -3654,7 +3667,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -3689,7 +3702,7 @@
         <v>0.98431372549019602</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3773,8 +3786,8 @@
         <v>0.46862745098039199</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1">
-      <c r="A60" t="s">
+    <row r="60" spans="1:11">
+      <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E60">
@@ -3799,7 +3812,7 @@
         <v>0.97450980392156805</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3825,8 +3838,8 @@
         <v>0.89215686274509798</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1">
-      <c r="A62" t="s">
+    <row r="62" spans="1:11">
+      <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E62">
@@ -3851,7 +3864,7 @@
         <v>0.98431372549019602</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3874,7 +3887,7 @@
         <v>0.91960784313725397</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3897,8 +3910,8 @@
         <v>0.98627450980392095</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1">
-      <c r="A65" t="s">
+    <row r="65" spans="1:11">
+      <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
       <c r="F65">
@@ -3920,7 +3933,7 @@
         <v>0.98823529411764699</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1">
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3943,7 +3956,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1">
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3966,8 +3979,8 @@
         <v>0.91764705882352904</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1">
-      <c r="A68" t="s">
+    <row r="68" spans="1:11">
+      <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F68">
@@ -3989,7 +4002,7 @@
         <v>0.99019607843137203</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1">
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -4009,8 +4022,8 @@
         <v>0.85882352941176399</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1">
-      <c r="A70" t="s">
+    <row r="70" spans="1:11">
+      <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
       <c r="G70">
@@ -4029,7 +4042,7 @@
         <v>0.92549019607843097</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1">
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -4049,7 +4062,7 @@
         <v>0.92745098039215601</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -4069,8 +4082,8 @@
         <v>0.96862745098039205</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1">
-      <c r="A73" t="s">
+    <row r="73" spans="1:11">
+      <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
       <c r="G73">
@@ -4089,7 +4102,7 @@
         <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1">
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4109,7 +4122,7 @@
         <v>0.51568627450980398</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -4129,8 +4142,8 @@
         <v>0.69215686274509802</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1">
-      <c r="A76" t="s">
+    <row r="76" spans="1:11">
+      <c r="A76" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H76">
@@ -4146,7 +4159,7 @@
         <v>0.87254901960784303</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1">
+    <row r="77" spans="1:11">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -4174,7 +4187,7 @@
         <v>0.22128851540616201</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1">
+    <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -4188,7 +4201,7 @@
         <v>0.98639455782312901</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1">
+    <row r="80" spans="1:11">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -4216,7 +4229,7 @@
         <v>0.135265700483091</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1">
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -4230,7 +4243,7 @@
         <v>0.71165644171779097</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -4265,7 +4278,7 @@
         <v>0.90980392156862699</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1">
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -4300,7 +4313,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1">
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -4335,7 +4348,7 @@
         <v>0.93529411764705805</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1">
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -4370,7 +4383,7 @@
         <v>0.99215686274509796</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -4440,7 +4453,7 @@
         <v>0.28823529411764698</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1">
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -4475,7 +4488,7 @@
         <v>0.96078431372549</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1">
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -4510,7 +4523,7 @@
         <v>0.97647058823529398</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1">
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -4545,7 +4558,7 @@
         <v>0.99215686274509796</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1">
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -4580,7 +4593,7 @@
         <v>0.86274509803921495</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1">
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -4615,7 +4628,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1">
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -4650,7 +4663,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1">
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -4685,8 +4698,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1">
-      <c r="A96" t="s">
+    <row r="96" spans="1:11">
+      <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
       <c r="D96">
@@ -4714,7 +4727,7 @@
         <v>0.94313725490195999</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1">
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -4743,7 +4756,7 @@
         <v>0.98823529411764699</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1">
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -4772,7 +4785,7 @@
         <v>0.88627450980392097</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1">
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -4801,8 +4814,8 @@
         <v>0.98431372549019602</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1">
-      <c r="A100" t="s">
+    <row r="100" spans="1:11">
+      <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
       <c r="D100">
@@ -4856,7 +4869,7 @@
         <v>0.48235294117646998</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1">
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -4882,7 +4895,7 @@
         <v>0.98235294117646998</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1">
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -4934,7 +4947,7 @@
         <v>0.43921568627450902</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1">
+    <row r="105" spans="1:11">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -4960,7 +4973,7 @@
         <v>0.84509803921568605</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1">
+    <row r="106" spans="1:11">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -4986,7 +4999,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1">
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -5003,7 +5016,7 @@
         <v>0.97254901960784301</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1">
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -5029,7 +5042,7 @@
         <v>0.915686274509803</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1">
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -5055,7 +5068,7 @@
         <v>0.90784313725490196</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1">
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -5081,7 +5094,7 @@
         <v>0.99215686274509796</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1">
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -5107,7 +5120,7 @@
         <v>0.98235294117646998</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1">
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -5133,7 +5146,7 @@
         <v>0.95882352941176396</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1">
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -5159,8 +5172,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1">
-      <c r="A114" t="s">
+    <row r="114" spans="1:11">
+      <c r="A114" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E114">
@@ -5186,7 +5199,7 @@
       </c>
     </row>
     <row r="115" spans="1:11">
-      <c r="A115" t="s">
+      <c r="A115" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E115">
@@ -5211,7 +5224,7 @@
         <v>0.40196078431372501</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1">
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -5234,8 +5247,8 @@
         <v>0.94705882352941095</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1">
-      <c r="A117" t="s">
+    <row r="117" spans="1:11">
+      <c r="A117" s="2" t="s">
         <v>115</v>
       </c>
       <c r="F117">
@@ -5280,7 +5293,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1">
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -5303,7 +5316,7 @@
         <v>0.90392156862745099</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1">
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -5326,7 +5339,7 @@
         <v>0.837254901960784</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1">
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -5341,7 +5354,7 @@
       </c>
     </row>
     <row r="122" spans="1:11">
-      <c r="A122" t="s">
+      <c r="A122" s="3" t="s">
         <v>120</v>
       </c>
       <c r="F122">
@@ -5363,7 +5376,7 @@
         <v>0.35882352941176399</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1">
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -5386,7 +5399,7 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1">
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -5406,8 +5419,8 @@
         <v>0.80196078431372497</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1">
-      <c r="A125" t="s">
+    <row r="125" spans="1:11">
+      <c r="A125" s="2" t="s">
         <v>123</v>
       </c>
       <c r="G125">
@@ -5426,7 +5439,7 @@
         <v>0.97254901960784301</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1">
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -5446,8 +5459,8 @@
         <v>0.71176470588235297</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1">
-      <c r="A127" t="s">
+    <row r="127" spans="1:11">
+      <c r="A127" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G127">
@@ -5466,8 +5479,8 @@
         <v>0.96274509803921504</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1">
-      <c r="A128" t="s">
+    <row r="128" spans="1:11">
+      <c r="A128" s="2" t="s">
         <v>126</v>
       </c>
       <c r="G128">
@@ -5486,8 +5499,8 @@
         <v>0.75882352941176401</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1">
-      <c r="A129" t="s">
+    <row r="129" spans="1:11">
+      <c r="A129" s="2" t="s">
         <v>127</v>
       </c>
       <c r="G129">
@@ -5506,7 +5519,7 @@
         <v>0.93137254901960698</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1">
+    <row r="130" spans="1:11">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -5526,7 +5539,7 @@
         <v>0.85882352941176399</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1">
+    <row r="131" spans="1:11">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -5546,7 +5559,7 @@
         <v>0.96666666666666601</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1">
+    <row r="132" spans="1:11">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -5566,7 +5579,7 @@
         <v>0.876470588235294</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1">
+    <row r="133" spans="1:11">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -5586,7 +5599,7 @@
         <v>0.915686274509803</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1">
+    <row r="134" spans="1:11">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -5606,7 +5619,7 @@
         <v>0.54313725490195996</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1">
+    <row r="135" spans="1:11">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -5626,8 +5639,8 @@
         <v>0.85098039215686205</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1">
-      <c r="A136" t="s">
+    <row r="136" spans="1:11">
+      <c r="A136" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G136">
@@ -5646,7 +5659,7 @@
         <v>0.93529411764705805</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1">
+    <row r="137" spans="1:11">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -5666,7 +5679,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1">
+    <row r="138" spans="1:11">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -5686,7 +5699,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1">
+    <row r="139" spans="1:11">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -5706,7 +5719,7 @@
         <v>0.95882352941176396</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1">
+    <row r="140" spans="1:11">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -5726,7 +5739,7 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1">
+    <row r="141" spans="1:11">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -5746,8 +5759,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1">
-      <c r="A142" t="s">
+    <row r="142" spans="1:11">
+      <c r="A142" s="2" t="s">
         <v>140</v>
       </c>
       <c r="G142">
@@ -5766,7 +5779,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1">
+    <row r="143" spans="1:11">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -5786,7 +5799,7 @@
         <v>0.97450980392156805</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1">
+    <row r="144" spans="1:11">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -5806,7 +5819,7 @@
         <v>0.81568627450980302</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1">
+    <row r="145" spans="1:11">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -5823,7 +5836,7 @@
         <v>0.77058823529411702</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1">
+    <row r="146" spans="1:11">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -5840,7 +5853,7 @@
         <v>0.99545454545454504</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1">
+    <row r="147" spans="1:11">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -5857,8 +5870,8 @@
         <v>0.75961538461538403</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1">
-      <c r="A148" t="s">
+    <row r="148" spans="1:11">
+      <c r="A148" s="2" t="s">
         <v>146</v>
       </c>
       <c r="H148">
@@ -5875,7 +5888,7 @@
       </c>
     </row>
     <row r="149" spans="1:11">
-      <c r="A149" t="s">
+      <c r="A149" s="3" t="s">
         <v>147</v>
       </c>
       <c r="I149">
@@ -5888,7 +5901,7 @@
         <v>0.19680851063829699</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1">
+    <row r="150" spans="1:11">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -5902,7 +5915,7 @@
         <v>0.90625</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1">
+    <row r="151" spans="1:11">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -5916,8 +5929,8 @@
         <v>0.80769230769230704</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1">
-      <c r="A152" t="s">
+    <row r="152" spans="1:11">
+      <c r="A152" s="2" t="s">
         <v>150</v>
       </c>
       <c r="I152">
@@ -5930,7 +5943,7 @@
         <v>0.86186186186186098</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1">
+    <row r="153" spans="1:11">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -5944,7 +5957,7 @@
         <v>0.80421686746987897</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1">
+    <row r="154" spans="1:11">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -5958,8 +5971,8 @@
         <v>0.70212765957446799</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1">
-      <c r="A155" t="s">
+    <row r="155" spans="1:11">
+      <c r="A155" s="2" t="s">
         <v>153</v>
       </c>
       <c r="I155">
@@ -5972,7 +5985,7 @@
         <v>0.996835443037974</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1">
+    <row r="156" spans="1:11">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -5986,7 +5999,7 @@
         <v>0.94637223974763396</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1">
+    <row r="157" spans="1:11">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -6000,8 +6013,8 @@
         <v>0.99065420560747597</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1">
-      <c r="A158" t="s">
+    <row r="158" spans="1:11">
+      <c r="A158" s="2" t="s">
         <v>156</v>
       </c>
       <c r="I158">
@@ -6014,7 +6027,7 @@
         <v>0.86779661016949095</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1">
+    <row r="159" spans="1:11">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -6042,7 +6055,7 @@
         <v>0.196721311475409</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1">
+    <row r="161" spans="1:11">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -6070,7 +6083,7 @@
         <v>0.488151658767772</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1">
+    <row r="163" spans="1:11">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -6084,7 +6097,7 @@
         <v>0.62135922330097004</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1">
+    <row r="164" spans="1:11">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -6098,7 +6111,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1">
+    <row r="165" spans="1:11">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -6133,7 +6146,7 @@
         <v>0.86470588235294099</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1">
+    <row r="166" spans="1:11">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -6203,7 +6216,7 @@
         <v>0.480392156862745</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1">
+    <row r="168" spans="1:11">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -6238,7 +6251,7 @@
         <v>0.79411764705882304</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1">
+    <row r="169" spans="1:11">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -6273,7 +6286,7 @@
         <v>0.93137254901960698</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1">
+    <row r="170" spans="1:11">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -6308,7 +6321,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1">
+    <row r="171" spans="1:11">
       <c r="A171" t="s">
         <v>169</v>
       </c>
@@ -6343,8 +6356,8 @@
         <v>0.95686274509803904</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1">
-      <c r="A172" t="s">
+    <row r="172" spans="1:11">
+      <c r="A172" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B172">
@@ -6378,7 +6391,7 @@
         <v>0.79803921568627401</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1">
+    <row r="173" spans="1:11">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -6413,7 +6426,7 @@
         <v>0.89607843137254894</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1">
+    <row r="174" spans="1:11">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -6448,7 +6461,7 @@
         <v>0.96470588235294097</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1">
+    <row r="175" spans="1:11">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -6483,8 +6496,8 @@
         <v>0.64509803921568598</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1">
-      <c r="A176" t="s">
+    <row r="176" spans="1:11">
+      <c r="A176" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B176">
@@ -6518,7 +6531,7 @@
         <v>0.96862745098039205</v>
       </c>
     </row>
-    <row r="177" spans="1:11" hidden="1">
+    <row r="177" spans="1:11">
       <c r="A177" t="s">
         <v>175</v>
       </c>
@@ -6553,7 +6566,7 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1">
+    <row r="178" spans="1:11">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -6620,8 +6633,8 @@
         <v>0.237254901960784</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1">
-      <c r="A180" t="s">
+    <row r="180" spans="1:11">
+      <c r="A180" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B180">
@@ -6691,7 +6704,7 @@
       </c>
     </row>
     <row r="182" spans="1:11">
-      <c r="A182" t="s">
+      <c r="A182" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B182">
@@ -6725,7 +6738,7 @@
         <v>0.19019607843137201</v>
       </c>
     </row>
-    <row r="183" spans="1:11" hidden="1">
+    <row r="183" spans="1:11">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -6760,7 +6773,7 @@
         <v>0.81176470588235194</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1">
+    <row r="184" spans="1:11">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -6795,8 +6808,8 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1">
-      <c r="A185" t="s">
+    <row r="185" spans="1:11">
+      <c r="A185" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B185">
@@ -6830,7 +6843,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1">
+    <row r="186" spans="1:11">
       <c r="A186" t="s">
         <v>184</v>
       </c>
@@ -6865,8 +6878,8 @@
         <v>0.954901960784313</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1">
-      <c r="A187" t="s">
+    <row r="187" spans="1:11">
+      <c r="A187" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B187">
@@ -6900,7 +6913,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1">
+    <row r="188" spans="1:11">
       <c r="A188" t="s">
         <v>186</v>
       </c>
@@ -6936,7 +6949,7 @@
       </c>
     </row>
     <row r="189" spans="1:11">
-      <c r="A189" t="s">
+      <c r="A189" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B189">
@@ -6970,7 +6983,7 @@
         <v>0.24901960784313701</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1">
+    <row r="190" spans="1:11">
       <c r="A190" t="s">
         <v>188</v>
       </c>
@@ -7005,7 +7018,7 @@
         <v>0.98431372549019602</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1">
+    <row r="191" spans="1:11">
       <c r="A191" t="s">
         <v>189</v>
       </c>
@@ -7040,7 +7053,7 @@
         <v>0.99215686274509796</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1">
+    <row r="192" spans="1:11">
       <c r="A192" t="s">
         <v>190</v>
       </c>
@@ -7075,7 +7088,7 @@
         <v>0.92745098039215601</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1">
+    <row r="193" spans="1:11">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -7145,7 +7158,7 @@
         <v>0.27058823529411702</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1">
+    <row r="195" spans="1:11">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -7180,7 +7193,7 @@
         <v>0.95686274509803904</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1">
+    <row r="196" spans="1:11">
       <c r="A196" t="s">
         <v>194</v>
       </c>
@@ -7215,7 +7228,7 @@
         <v>0.96274509803921504</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1">
+    <row r="197" spans="1:11">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -7250,8 +7263,8 @@
         <v>0.89019607843137205</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1">
-      <c r="A198" t="s">
+    <row r="198" spans="1:11">
+      <c r="A198" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B198">
@@ -7285,7 +7298,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1">
+    <row r="199" spans="1:11">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -7355,7 +7368,7 @@
         <v>0.49215686274509801</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1">
+    <row r="201" spans="1:11">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -7390,7 +7403,7 @@
         <v>0.99019607843137203</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1">
+    <row r="202" spans="1:11">
       <c r="A202" t="s">
         <v>200</v>
       </c>
@@ -7425,7 +7438,7 @@
         <v>0.95294117647058796</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1">
+    <row r="203" spans="1:11">
       <c r="A203" t="s">
         <v>201</v>
       </c>
@@ -7460,7 +7473,7 @@
         <v>0.93725490196078398</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1">
+    <row r="204" spans="1:11">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -7495,7 +7508,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1">
+    <row r="205" spans="1:11">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -7565,7 +7578,7 @@
         <v>0.43921568627450902</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1">
+    <row r="207" spans="1:11">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -7600,7 +7613,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1">
+    <row r="208" spans="1:11">
       <c r="A208" t="s">
         <v>206</v>
       </c>
@@ -7614,7 +7627,7 @@
         <v>0.93375394321766503</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1">
+    <row r="209" spans="1:11">
       <c r="A209" t="s">
         <v>207</v>
       </c>
@@ -7669,7 +7682,7 @@
         <v>0.370588235294117</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1">
+    <row r="211" spans="1:11">
       <c r="A211" t="s">
         <v>209</v>
       </c>
@@ -7768,7 +7781,7 @@
         <v>8.6274509803921498E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1">
+    <row r="214" spans="1:11">
       <c r="A214" t="s">
         <v>212</v>
       </c>
@@ -7782,7 +7795,7 @@
         <v>0.50249999999999995</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1">
+    <row r="215" spans="1:11">
       <c r="A215" t="s">
         <v>213</v>
       </c>
@@ -7802,7 +7815,7 @@
         <v>0.99019607843137203</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1">
+    <row r="216" spans="1:11">
       <c r="A216" t="s">
         <v>214</v>
       </c>
@@ -7839,7 +7852,7 @@
         <v>0.26706231454005902</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1">
+    <row r="218" spans="1:11">
       <c r="A218" t="s">
         <v>216</v>
       </c>
@@ -7876,8 +7889,8 @@
         <v>0.22156862745097999</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1">
-      <c r="A220" t="s">
+    <row r="220" spans="1:11">
+      <c r="A220" s="3" t="s">
         <v>218</v>
       </c>
       <c r="F220">
@@ -7899,8 +7912,8 @@
         <v>0.50980392156862697</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1">
-      <c r="A221" t="s">
+    <row r="221" spans="1:11">
+      <c r="A221" s="2" t="s">
         <v>219</v>
       </c>
       <c r="E221">
@@ -7925,7 +7938,7 @@
         <v>0.97450980392156805</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1">
+    <row r="222" spans="1:11">
       <c r="A222" t="s">
         <v>220</v>
       </c>
@@ -7948,7 +7961,7 @@
         <v>0.93921568627450902</v>
       </c>
     </row>
-    <row r="223" spans="1:11" hidden="1">
+    <row r="223" spans="1:11">
       <c r="A223" t="s">
         <v>221</v>
       </c>
@@ -7962,7 +7975,7 @@
         <v>0.99056603773584895</v>
       </c>
     </row>
-    <row r="224" spans="1:11" hidden="1">
+    <row r="224" spans="1:11">
       <c r="A224" t="s">
         <v>222</v>
       </c>
@@ -7982,8 +7995,8 @@
         <v>0.80392156862745101</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1">
-      <c r="A225" t="s">
+    <row r="225" spans="1:11">
+      <c r="A225" s="2" t="s">
         <v>223</v>
       </c>
       <c r="D225">
@@ -8011,7 +8024,7 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1">
+    <row r="226" spans="1:11">
       <c r="A226" t="s">
         <v>224</v>
       </c>
@@ -8037,7 +8050,7 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1">
+    <row r="227" spans="1:11">
       <c r="A227" t="s">
         <v>225</v>
       </c>
@@ -8051,7 +8064,7 @@
         <v>0.99702380952380898</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1">
+    <row r="228" spans="1:11">
       <c r="A228" t="s">
         <v>226</v>
       </c>
@@ -8065,7 +8078,7 @@
         <v>0.64423076923076905</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1">
+    <row r="229" spans="1:11">
       <c r="A229" t="s">
         <v>227</v>
       </c>
@@ -8092,7 +8105,7 @@
       </c>
     </row>
     <row r="230" spans="1:11">
-      <c r="A230" t="s">
+      <c r="A230" s="3" t="s">
         <v>228</v>
       </c>
       <c r="G230">
@@ -8111,8 +8124,8 @@
         <v>0.35490196078431302</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1">
-      <c r="A231" t="s">
+    <row r="231" spans="1:11">
+      <c r="A231" s="2" t="s">
         <v>229</v>
       </c>
       <c r="D231">
@@ -8154,7 +8167,7 @@
         <v>0.17971014492753601</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1">
+    <row r="233" spans="1:11">
       <c r="A233" t="s">
         <v>231</v>
       </c>
@@ -8174,7 +8187,7 @@
         <v>0.91372549019607796</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1">
+    <row r="234" spans="1:11">
       <c r="A234" t="s">
         <v>232</v>
       </c>
@@ -8197,8 +8210,8 @@
         <v>0.79019607843137196</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1">
-      <c r="A235" t="s">
+    <row r="235" spans="1:11">
+      <c r="A235" s="2" t="s">
         <v>233</v>
       </c>
       <c r="G235">
@@ -8217,8 +8230,8 @@
         <v>0.96470588235294097</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1">
-      <c r="A236" t="s">
+    <row r="236" spans="1:11">
+      <c r="A236" s="2" t="s">
         <v>234</v>
       </c>
       <c r="G236">
@@ -8237,8 +8250,8 @@
         <v>0.99607843137254903</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1">
-      <c r="A237" t="s">
+    <row r="237" spans="1:11">
+      <c r="A237" s="2" t="s">
         <v>235</v>
       </c>
       <c r="G237">
@@ -8257,7 +8270,7 @@
         <v>0.67254901960784297</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1">
+    <row r="238" spans="1:11">
       <c r="A238" t="s">
         <v>236</v>
       </c>
@@ -8271,7 +8284,7 @@
         <v>0.949238578680203</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1">
+    <row r="239" spans="1:11">
       <c r="A239" t="s">
         <v>237</v>
       </c>
@@ -8317,8 +8330,8 @@
         <v>0.43137254901960698</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1">
-      <c r="A241" t="s">
+    <row r="241" spans="1:11">
+      <c r="A241" s="2" t="s">
         <v>239</v>
       </c>
       <c r="G241">
@@ -8337,8 +8350,8 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1">
-      <c r="A242" t="s">
+    <row r="242" spans="1:11">
+      <c r="A242" s="2" t="s">
         <v>240</v>
       </c>
       <c r="E242">
@@ -8363,7 +8376,7 @@
         <v>0.98235294117646998</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1">
+    <row r="243" spans="1:11">
       <c r="A243" t="s">
         <v>241</v>
       </c>
@@ -8403,7 +8416,7 @@
         <v>0.11764705882352899</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1">
+    <row r="245" spans="1:11">
       <c r="A245" t="s">
         <v>243</v>
       </c>
@@ -8420,8 +8433,8 @@
         <v>0.83529411764705797</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1">
-      <c r="A246" t="s">
+    <row r="246" spans="1:11">
+      <c r="A246" s="2" t="s">
         <v>244</v>
       </c>
       <c r="E246">
@@ -8446,7 +8459,7 @@
         <v>0.79019607843137196</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1">
+    <row r="247" spans="1:11">
       <c r="A247" t="s">
         <v>245</v>
       </c>
@@ -8460,8 +8473,8 @@
         <v>0.56310679611650405</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1">
-      <c r="A248" t="s">
+    <row r="248" spans="1:11">
+      <c r="A248" s="2" t="s">
         <v>246</v>
       </c>
       <c r="G248">
@@ -8480,8 +8493,8 @@
         <v>0.97647058823529398</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1">
-      <c r="A249" t="s">
+    <row r="249" spans="1:11">
+      <c r="A249" s="2" t="s">
         <v>247</v>
       </c>
       <c r="F249">
@@ -8503,8 +8516,8 @@
         <v>0.97647058823529398</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1">
-      <c r="A250" t="s">
+    <row r="250" spans="1:11">
+      <c r="A250" s="2" t="s">
         <v>248</v>
       </c>
       <c r="H250">
@@ -8520,7 +8533,7 @@
         <v>0.94117647058823495</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1">
+    <row r="251" spans="1:11">
       <c r="A251" t="s">
         <v>249</v>
       </c>
@@ -8534,8 +8547,8 @@
         <v>0.984615384615384</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1">
-      <c r="A252" t="s">
+    <row r="252" spans="1:11">
+      <c r="A252" s="2" t="s">
         <v>250</v>
       </c>
       <c r="G252">
@@ -8554,7 +8567,7 @@
         <v>0.97843137254901902</v>
       </c>
     </row>
-    <row r="253" spans="1:11" hidden="1">
+    <row r="253" spans="1:11">
       <c r="A253" t="s">
         <v>251</v>
       </c>
@@ -8568,8 +8581,8 @@
         <v>0.89754098360655699</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1">
-      <c r="A254" t="s">
+    <row r="254" spans="1:11">
+      <c r="A254" s="2" t="s">
         <v>252</v>
       </c>
       <c r="G254">
@@ -8588,7 +8601,7 @@
         <v>0.92941176470588205</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1">
+    <row r="255" spans="1:11">
       <c r="A255" t="s">
         <v>253</v>
       </c>
@@ -8608,7 +8621,7 @@
         <v>0.92941176470588205</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1">
+    <row r="256" spans="1:11">
       <c r="A256" t="s">
         <v>254</v>
       </c>
@@ -8648,7 +8661,7 @@
         <v>0.45294117647058801</v>
       </c>
     </row>
-    <row r="258" spans="1:11" hidden="1">
+    <row r="258" spans="1:11">
       <c r="A258" t="s">
         <v>256</v>
       </c>
@@ -8668,8 +8681,8 @@
         <v>0.90980392156862699</v>
       </c>
     </row>
-    <row r="259" spans="1:11" hidden="1">
-      <c r="A259" t="s">
+    <row r="259" spans="1:11">
+      <c r="A259" s="3" t="s">
         <v>257</v>
       </c>
       <c r="G259">
@@ -8688,7 +8701,7 @@
         <v>0.50196078431372504</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1">
+    <row r="260" spans="1:11">
       <c r="A260" t="s">
         <v>258</v>
       </c>
@@ -8711,7 +8724,7 @@
         <v>0.97058823529411697</v>
       </c>
     </row>
-    <row r="261" spans="1:11" hidden="1">
+    <row r="261" spans="1:11">
       <c r="A261" t="s">
         <v>259</v>
       </c>
@@ -8737,7 +8750,7 @@
         <v>0.77058823529411702</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1">
+    <row r="262" spans="1:11">
       <c r="A262" t="s">
         <v>260</v>
       </c>
@@ -8757,7 +8770,7 @@
         <v>0.99803921568627396</v>
       </c>
     </row>
-    <row r="263" spans="1:11" hidden="1">
+    <row r="263" spans="1:11">
       <c r="A263" t="s">
         <v>261</v>
       </c>
@@ -8771,7 +8784,7 @@
         <v>0.72388059701492502</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1">
+    <row r="264" spans="1:11">
       <c r="A264" t="s">
         <v>262</v>
       </c>
@@ -8794,7 +8807,7 @@
         <v>0.80784313725490198</v>
       </c>
     </row>
-    <row r="265" spans="1:11" hidden="1">
+    <row r="265" spans="1:11">
       <c r="A265" t="s">
         <v>263</v>
       </c>
@@ -8823,7 +8836,7 @@
         <v>0.95294117647058796</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1">
+    <row r="266" spans="1:11">
       <c r="A266" t="s">
         <v>264</v>
       </c>
@@ -8837,7 +8850,7 @@
         <v>0.89298892988929801</v>
       </c>
     </row>
-    <row r="267" spans="1:11" hidden="1">
+    <row r="267" spans="1:11">
       <c r="A267" t="s">
         <v>265</v>
       </c>
@@ -8851,7 +8864,7 @@
         <v>0.50553505535055299</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1">
+    <row r="268" spans="1:11">
       <c r="A268" t="s">
         <v>266</v>
       </c>
@@ -8879,7 +8892,7 @@
         <v>0.43542435424354198</v>
       </c>
     </row>
-    <row r="270" spans="1:11" hidden="1">
+    <row r="270" spans="1:11">
       <c r="A270" t="s">
         <v>268</v>
       </c>
@@ -8907,7 +8920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:11" hidden="1">
+    <row r="272" spans="1:11">
       <c r="A272" t="s">
         <v>270</v>
       </c>
@@ -8921,7 +8934,7 @@
         <v>0.94961240310077499</v>
       </c>
     </row>
-    <row r="273" spans="1:11" hidden="1">
+    <row r="273" spans="1:11">
       <c r="A273" t="s">
         <v>271</v>
       </c>
@@ -8935,7 +8948,7 @@
         <v>0.94708994708994698</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1">
+    <row r="274" spans="1:11">
       <c r="A274" t="s">
         <v>272</v>
       </c>
@@ -8963,7 +8976,7 @@
         <v>0.43646408839779</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1">
+    <row r="276" spans="1:11">
       <c r="A276" t="s">
         <v>274</v>
       </c>
@@ -8992,13 +9005,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K277" xr:uid="{75A6FE0F-ABED-4571-A256-B0E850D77F89}">
-    <filterColumn colId="10">
-      <customFilters>
-        <customFilter operator="lessThan" val="0.5"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K277" xr:uid="{75A6FE0F-ABED-4571-A256-B0E850D77F89}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>